<commit_message>
Update to new format Fix QuickCharts
</commit_message>
<xml_diff>
--- a/tests/fixtures/idmc_displacement_all_dataset.xlsx
+++ b/tests/fixtures/idmc_displacement_all_dataset.xlsx
@@ -34,10 +34,10 @@
     <t xml:space="preserve">Conflict Stock Displacement</t>
   </si>
   <si>
-    <t xml:space="preserve">Conflict New Displacements</t>
+    <t xml:space="preserve">Conflict Internal Displacements</t>
   </si>
   <si>
-    <t xml:space="preserve">Disaster New Displacements</t>
+    <t xml:space="preserve">Disaster Internal Displacements</t>
   </si>
   <si>
     <t xml:space="preserve">#country+code</t>
@@ -52,10 +52,10 @@
     <t xml:space="preserve">#affected+idps+ind+stock+conflict</t>
   </si>
   <si>
-    <t xml:space="preserve">#affected+idps+ind+newdisp+conflict</t>
+    <t xml:space="preserve">#affected+idps+ind+internaldisp+conflict</t>
   </si>
   <si>
-    <t xml:space="preserve">#affected+idps+ind+newdisp+disaster</t>
+    <t xml:space="preserve">#affected+idps+ind+internaldisp+disaster</t>
   </si>
   <si>
     <t xml:space="preserve">AB9</t>
@@ -167,31 +167,28 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:F8"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>